<commit_message>
discount method updated to ifrs17 standarts
</commit_message>
<xml_diff>
--- a/future_value.xlsx
+++ b/future_value.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eren/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eren\Desktop\Projects\discounted_cashflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EB5BDE-13C4-4D4C-B8C2-58893BEAD292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507333BA-7FD8-43E3-9696-90E83791ABA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa2" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Group</t>
   </si>
@@ -47,10 +47,16 @@
     <t>uoa2</t>
   </si>
   <si>
-    <t>uoa3</t>
-  </si>
-  <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -374,45 +380,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344448C0-5813-EF41-B935-311A4303076B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>10000</v>
+      <c r="B2">
+        <v>2007</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>16823445.68</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>15000</v>
+      <c r="B3">
+        <v>2014</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4005582.31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>20000</v>
-      </c>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
expandable summary data added.
</commit_message>
<xml_diff>
--- a/future_value.xlsx
+++ b/future_value.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eren\Desktop\Eren-Backup\Projects\discounted_cashflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eren/development/discounted_cf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A7DB0D-03A0-4DC3-B584-294E9C243E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2DCD67-B720-E848-B393-99328586B936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa2" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -392,15 +391,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,51 +413,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>2023</v>
+        <v>2007</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>25059631</v>
+        <v>16823445.68</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>2007</v>
+        <v>2014</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2">
-        <v>16823445.68</v>
+        <v>4005582.31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>2014</v>
+        <v>2023</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
-        <v>4005582.31</v>
+        <v>20098221.34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>2023</v>
@@ -467,7 +466,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2">
-        <v>20098221.34</v>
+        <v>25059631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>